<commit_message>
chore: update test data
</commit_message>
<xml_diff>
--- a/assets/xlsx-upload-template.xlsx
+++ b/assets/xlsx-upload-template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>EmpID</t>
   </si>
@@ -28,46 +28,16 @@
     <t>2013-11-01</t>
   </si>
   <si>
-    <t>2014-01-05</t>
+    <t>2013-11-10</t>
   </si>
   <si>
-    <t>2012-05-16</t>
+    <t>2013-11-15</t>
   </si>
   <si>
-    <t>NULL</t>
+    <t>2013-11-05</t>
   </si>
   <si>
-    <t>2009-01-01</t>
-  </si>
-  <si>
-    <t>2011-04-27</t>
-  </si>
-  <si>
-    <t>2015-08-20</t>
-  </si>
-  <si>
-    <t>2016-02-10</t>
-  </si>
-  <si>
-    <t>2016-03-12</t>
-  </si>
-  <si>
-    <t>2018-09-30</t>
-  </si>
-  <si>
-    <t>2017-06-03</t>
-  </si>
-  <si>
-    <t>2019-12-15</t>
-  </si>
-  <si>
-    <t>2018-11-15</t>
-  </si>
-  <si>
-    <t>2020-02-28</t>
-  </si>
-  <si>
-    <t>2022-07-20</t>
+    <t>2013-11-09</t>
   </si>
 </sst>
 </file>
@@ -364,98 +334,74 @@
         <v>218.0</v>
       </c>
       <c r="B3" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="B5" s="1">
         <v>10.0</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1">
+    <row r="6">
+      <c r="A6" s="1">
         <v>143.0</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B6" s="1">
         <v>10.0</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1">
-        <v>325.0</v>
-      </c>
-      <c r="B5" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1">
-        <v>218.0</v>
-      </c>
-      <c r="B6" s="1">
-        <v>25.0</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="7">
-      <c r="A7" s="1">
-        <v>743.0</v>
-      </c>
-      <c r="B7" s="1">
-        <v>18.0</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="1">
-        <v>522.0</v>
-      </c>
-      <c r="B8" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="1">
-        <v>621.0</v>
-      </c>
-      <c r="B9" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
     </row>
     <row r="10">
       <c r="C10" s="3"/>

</xml_diff>